<commit_message>
Dokumentation: Realisieren fast abgeschlossen
- Konzept- und Prinzipskizze nachgetragen
- Berechnungen gemacht
- Dokumentation nachgetragen
</commit_message>
<xml_diff>
--- a/10_Aufgabenstellung/Bewertungsbogen Pflanzenwagen.xlsx
+++ b/10_Aufgabenstellung/Bewertungsbogen Pflanzenwagen.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209F04F2-65BE-4002-A80E-87AA98EA8090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62CE27E-DC22-4E1A-8022-F35FD4397F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>Massstab</t>
   </si>
   <si>
-    <t>vollständig</t>
-  </si>
-  <si>
     <t>Montage- &amp; Betriebsanleitung</t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     <t>Maschinenelemente (keine Zeichnungen)</t>
   </si>
   <si>
-    <t xml:space="preserve">              "            Handelsteile</t>
-  </si>
-  <si>
     <t>richtig eingesetzt</t>
   </si>
   <si>
@@ -353,24 +347,13 @@
     <t>Die Noten wurde nach dieser Formel berechnet (max. Punktzahl ist 58)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Pflichtenheft</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, Prinzipzkizzen</t>
-    </r>
+    <t>Pflichtenheft, Prinzipzkizzen</t>
+  </si>
+  <si>
+    <t>vollständig (Zeichnung?)</t>
+  </si>
+  <si>
+    <t>Handelsteile</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1072,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1363,6 +1346,13 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1378,11 +1368,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1777,8 +1766,8 @@
   </sheetPr>
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,11 +1784,11 @@
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="125" t="s">
+      <c r="D1" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
       <c r="G1" s="41" t="s">
         <v>1</v>
       </c>
@@ -1808,21 +1797,21 @@
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="124" t="s">
+      <c r="D2" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
       <c r="G2" s="120" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="122"/>
-      <c r="C3" s="123"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="126"/>
       <c r="D3" s="34" t="s">
         <v>5</v>
       </c>
@@ -1874,8 +1863,8 @@
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>106</v>
+      <c r="B6" s="123" t="s">
+        <v>104</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="49"/>
@@ -1889,7 +1878,7 @@
     </row>
     <row r="7" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="126" t="s">
+      <c r="B7" s="121" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="9"/>
@@ -1919,7 +1908,7 @@
     </row>
     <row r="9" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="106"/>
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="129" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="108"/>
@@ -1932,7 +1921,7 @@
     </row>
     <row r="10" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
-      <c r="B10" s="126" t="s">
+      <c r="B10" s="121" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="9"/>
@@ -1946,10 +1935,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="127" t="s">
+      <c r="A11" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="128" t="s">
+      <c r="B11" s="123" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="10"/>
@@ -2012,10 +2001,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="126" t="s">
+      <c r="B15" s="121" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="9"/>
@@ -2029,7 +2018,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="122" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="12"/>
@@ -2044,10 +2033,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="127" t="s">
+      <c r="A17" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="121" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="9"/>
@@ -2062,7 +2051,7 @@
     </row>
     <row r="18" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="128" t="s">
+      <c r="B18" s="123" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="10"/>
@@ -2077,7 +2066,7 @@
     </row>
     <row r="19" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
-      <c r="B19" s="126" t="s">
+      <c r="B19" s="121" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="9"/>
@@ -2125,10 +2114,10 @@
       <c r="I21" s="83"/>
     </row>
     <row r="22" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="128" t="s">
+      <c r="B22" s="123" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="10"/>
@@ -2143,7 +2132,7 @@
     </row>
     <row r="23" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="121" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="9"/>
@@ -2205,7 +2194,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="127" t="s">
+      <c r="A27" s="122" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="3"/>
@@ -2219,7 +2208,7 @@
     </row>
     <row r="28" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
-      <c r="B28" s="128" t="s">
+      <c r="B28" s="123" t="s">
         <v>37</v>
       </c>
       <c r="C28" s="10"/>
@@ -2234,7 +2223,7 @@
     </row>
     <row r="29" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
-      <c r="B29" s="126" t="s">
+      <c r="B29" s="121" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="9"/>
@@ -2249,7 +2238,7 @@
     </row>
     <row r="30" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="123" t="s">
         <v>39</v>
       </c>
       <c r="C30" s="10"/>
@@ -2264,7 +2253,7 @@
     </row>
     <row r="31" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="121" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="9"/>
@@ -2281,7 +2270,7 @@
       <c r="A32" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="123" t="s">
         <v>42</v>
       </c>
       <c r="C32" s="10"/>
@@ -2296,7 +2285,7 @@
     </row>
     <row r="33" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="121" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="9"/>
@@ -2311,7 +2300,7 @@
     </row>
     <row r="34" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="123" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="10"/>
@@ -2326,7 +2315,7 @@
     </row>
     <row r="35" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="130" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="22"/>
@@ -2342,7 +2331,7 @@
     <row r="36" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
       <c r="B36" s="13" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="53"/>
@@ -2375,10 +2364,10 @@
     </row>
     <row r="38" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="28" t="s">
         <v>45</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>46</v>
       </c>
       <c r="C38" s="99" t="s">
         <v>20</v>
@@ -2396,10 +2385,10 @@
     </row>
     <row r="39" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="62"/>
@@ -2412,7 +2401,7 @@
     <row r="40" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="49"/>
@@ -2427,7 +2416,7 @@
     <row r="41" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="49"/>
@@ -2442,7 +2431,7 @@
     <row r="42" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="49"/>
@@ -2456,7 +2445,7 @@
       <c r="A43" s="11"/>
       <c r="B43" s="12"/>
       <c r="C43" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D43" s="49"/>
       <c r="E43" s="59"/>
@@ -2471,7 +2460,7 @@
       <c r="A44" s="11"/>
       <c r="B44" s="3"/>
       <c r="C44" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D44" s="49"/>
       <c r="E44" s="59"/>
@@ -2486,7 +2475,7 @@
       <c r="A45" s="11"/>
       <c r="B45" s="12"/>
       <c r="C45" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D45" s="49"/>
       <c r="E45" s="59"/>
@@ -2500,7 +2489,7 @@
     <row r="46" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="49"/>
@@ -2513,10 +2502,10 @@
     <row r="47" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="12" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D47" s="49"/>
       <c r="E47" s="59"/>
@@ -2530,7 +2519,7 @@
     <row r="48" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="49"/>
@@ -2545,7 +2534,7 @@
     <row r="49" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="49"/>
@@ -2560,7 +2549,7 @@
     <row r="50" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C50" s="9"/>
       <c r="D50" s="49"/>
@@ -2575,7 +2564,7 @@
     <row r="51" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11"/>
       <c r="B51" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="53"/>
@@ -2608,7 +2597,7 @@
     </row>
     <row r="53" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>35</v>
@@ -2624,7 +2613,7 @@
     <row r="54" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C54" s="22"/>
       <c r="D54" s="62"/>
@@ -2639,7 +2628,7 @@
     <row r="55" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="B55" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="49"/>
@@ -2653,7 +2642,7 @@
       <c r="A56" s="11"/>
       <c r="B56" s="12"/>
       <c r="C56" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D56" s="49"/>
       <c r="E56" s="59"/>
@@ -2668,7 +2657,7 @@
       <c r="A57" s="11"/>
       <c r="B57" s="3"/>
       <c r="C57" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D57" s="49"/>
       <c r="E57" s="59"/>
@@ -2683,7 +2672,7 @@
       <c r="A58" s="11"/>
       <c r="B58" s="12"/>
       <c r="C58" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D58" s="49"/>
       <c r="E58" s="59"/>
@@ -2697,7 +2686,7 @@
     <row r="59" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C59" s="9"/>
       <c r="D59" s="49"/>
@@ -2711,7 +2700,7 @@
       <c r="A60" s="11"/>
       <c r="B60" s="12"/>
       <c r="C60" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D60" s="49"/>
       <c r="E60" s="59"/>
@@ -2726,7 +2715,7 @@
       <c r="A61" s="11"/>
       <c r="B61" s="3"/>
       <c r="C61" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D61" s="49"/>
       <c r="E61" s="59"/>
@@ -2740,7 +2729,7 @@
     <row r="62" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C62" s="10"/>
       <c r="D62" s="49"/>
@@ -2755,7 +2744,7 @@
     <row r="63" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="49"/>
@@ -2770,7 +2759,7 @@
     <row r="64" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11"/>
       <c r="B64" s="107" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C64" s="108"/>
       <c r="D64" s="114"/>
@@ -2801,7 +2790,7 @@
     </row>
     <row r="66" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>35</v>
@@ -2817,7 +2806,7 @@
     <row r="67" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="49"/>
@@ -2832,7 +2821,7 @@
     <row r="68" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C68" s="10"/>
       <c r="D68" s="49"/>
@@ -2847,7 +2836,7 @@
     <row r="69" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C69" s="22"/>
       <c r="D69" s="49"/>
@@ -2862,7 +2851,7 @@
     <row r="70" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="49"/>
@@ -2877,7 +2866,7 @@
     <row r="71" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="39"/>
       <c r="B71" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C71" s="20"/>
       <c r="D71" s="51"/>
@@ -2892,7 +2881,7 @@
     <row r="72" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="31"/>
       <c r="B72" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C72" s="86"/>
       <c r="D72" s="54"/>
@@ -2925,10 +2914,10 @@
     </row>
     <row r="74" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B74" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C74" s="22"/>
       <c r="D74" s="62"/>
@@ -2941,7 +2930,7 @@
     <row r="75" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C75" s="10"/>
       <c r="D75" s="49"/>
@@ -2956,7 +2945,7 @@
     <row r="76" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="49"/>
@@ -2971,7 +2960,7 @@
     <row r="77" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11"/>
       <c r="B77" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="52"/>
@@ -3002,10 +2991,10 @@
     </row>
     <row r="79" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C79" s="17"/>
       <c r="D79" s="46"/>
@@ -3018,7 +3007,7 @@
     <row r="80" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C80" s="10"/>
       <c r="D80" s="49"/>
@@ -3033,7 +3022,7 @@
     <row r="81" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="11"/>
       <c r="B81" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C81" s="9"/>
       <c r="D81" s="53"/>
@@ -3065,10 +3054,10 @@
     </row>
     <row r="83" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C83" s="17"/>
       <c r="D83" s="62"/>
@@ -3081,7 +3070,7 @@
     <row r="84" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C84" s="10"/>
       <c r="D84" s="49"/>
@@ -3096,7 +3085,7 @@
     <row r="85" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="24"/>
       <c r="B85" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C85" s="26"/>
       <c r="D85" s="60"/>
@@ -3129,10 +3118,10 @@
     </row>
     <row r="87" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C87" s="17"/>
       <c r="D87" s="46"/>
@@ -3159,7 +3148,7 @@
     </row>
     <row r="89" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="9"/>
@@ -3173,7 +3162,7 @@
     <row r="90" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11"/>
       <c r="B90" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C90" s="10"/>
       <c r="D90" s="49"/>
@@ -3187,7 +3176,7 @@
     </row>
     <row r="91" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="9"/>
@@ -3201,7 +3190,7 @@
     <row r="92" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11"/>
       <c r="B92" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C92" s="10"/>
       <c r="D92" s="49"/>
@@ -3216,7 +3205,7 @@
     <row r="93" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="11"/>
       <c r="B93" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C93" s="9"/>
       <c r="D93" s="49"/>
@@ -3231,7 +3220,7 @@
     <row r="94" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="11"/>
       <c r="B94" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="49"/>
@@ -3245,7 +3234,7 @@
     </row>
     <row r="95" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="9"/>
@@ -3259,7 +3248,7 @@
     <row r="96" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="11"/>
       <c r="B96" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C96" s="10"/>
       <c r="D96" s="49"/>
@@ -3274,7 +3263,7 @@
     <row r="97" spans="1:9" ht="21.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="11"/>
       <c r="B97" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C97" s="9"/>
       <c r="D97" s="49"/>
@@ -3289,7 +3278,7 @@
     <row r="98" spans="1:9" ht="21.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="11"/>
       <c r="B98" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C98" s="9"/>
       <c r="D98" s="53"/>
@@ -3324,7 +3313,7 @@
       <c r="A100" s="11"/>
       <c r="B100" s="3"/>
       <c r="C100" s="103" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D100" s="79"/>
       <c r="E100" s="80"/>
@@ -3341,17 +3330,17 @@
     </row>
     <row r="101" spans="1:9" ht="29.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A101" s="33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B101" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C101" s="77"/>
       <c r="D101" s="26"/>
       <c r="E101" s="76"/>
       <c r="F101" s="78"/>
       <c r="G101" s="43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H101" s="92"/>
       <c r="I101" s="95"/>
@@ -3367,7 +3356,7 @@
     </row>
     <row r="104" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="G104" s="119" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3411,15 +3400,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010080D5ACB5D9A5C547A8A8A6B4DC26C831" ma:contentTypeVersion="36" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8d7a45047883c5514381d1f862dec088">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ec5a2d1-872f-46b3-83ae-e3f81ffd97c7" xmlns:ns3="5954586a-bae9-408a-b7c4-5e38477065a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="34aeb3f1ae918c8f1a8c56ed432b74e6" ns2:_="" ns3:_="">
     <xsd:import namespace="4ec5a2d1-872f-46b3-83ae-e3f81ffd97c7"/>
@@ -3850,6 +3830,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3907,14 +3896,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A686A6BC-AD03-4242-A509-915B93A7FC06}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCB0D0B6-0EEB-45DB-9889-96243CF72E68}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3933,6 +3914,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A686A6BC-AD03-4242-A509-915B93A7FC06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{753FD138-AAAB-46CD-93E9-84A3CCF0DAEC}">
   <ds:schemaRefs>

</xml_diff>